<commit_message>
added first name object to the test
</commit_message>
<xml_diff>
--- a/test_data/TestData.xlsx
+++ b/test_data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="8535" windowHeight="4620" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="8535" windowHeight="4620"/>
   </bookViews>
   <sheets>
     <sheet name="BadSignin" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>abcd</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -389,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,7 +418,7 @@
     <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -408,61 +426,79 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1">
         <v>1991</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1">
         <v>1992</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1">
         <v>1993</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1">
         <v>1994</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
         <v>1995</v>
       </c>
     </row>
@@ -475,7 +511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>